<commit_message>
Perform tests and choose heuristic
</commit_message>
<xml_diff>
--- a/model_results.xlsx
+++ b/model_results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
   <si>
     <t>In the move.</t>
   </si>
@@ -33,6 +33,15 @@
   </si>
   <si>
     <t>Two moves ahead.</t>
+  </si>
+  <si>
+    <t>Divide player moves by opponents moves.</t>
+  </si>
+  <si>
+    <t>ID_Improved</t>
+  </si>
+  <si>
+    <t>Student</t>
   </si>
 </sst>
 </file>
@@ -68,8 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,20 +394,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>65.714285714285694</v>
       </c>
@@ -413,7 +423,7 @@
         <v>66.71428571428568</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>66.428571428571402</v>
       </c>
@@ -428,157 +438,508 @@
         <f>_xlfn.STDEV.S(B2:B21)</f>
         <v>4.0299629655568028</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>68.571428571428498</v>
       </c>
       <c r="B4">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>62.857142857142797</v>
       </c>
       <c r="B5">
         <v>71.428571428571402</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H5" s="1">
+        <v>65.714285714285694</v>
+      </c>
+      <c r="I5" s="1">
+        <v>62.857142857142797</v>
+      </c>
+      <c r="J5" s="1">
+        <v>68.571428571428498</v>
+      </c>
+      <c r="K5" s="1">
+        <v>65</v>
+      </c>
+      <c r="L5" s="1">
+        <v>67.142857142857096</v>
+      </c>
+      <c r="M5" s="1">
+        <v>58.571428571428498</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>65</v>
       </c>
       <c r="B6">
         <v>65.714285714285694</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H6" s="1">
+        <v>66.428571428571402</v>
+      </c>
+      <c r="I6" s="1">
+        <v>65</v>
+      </c>
+      <c r="J6" s="1">
+        <v>64.285714285714207</v>
+      </c>
+      <c r="K6" s="1">
+        <v>65</v>
+      </c>
+      <c r="L6" s="1">
+        <v>69.285714285714207</v>
+      </c>
+      <c r="M6" s="1">
+        <v>57.142857142857103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>63.571428571428498</v>
       </c>
       <c r="B7">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H7" s="1">
+        <v>68.571428571428498</v>
+      </c>
+      <c r="I7" s="1">
+        <v>60</v>
+      </c>
+      <c r="J7" s="1">
+        <v>69.285714285714207</v>
+      </c>
+      <c r="K7" s="1">
+        <v>70</v>
+      </c>
+      <c r="L7" s="1">
+        <v>70</v>
+      </c>
+      <c r="M7" s="1">
+        <v>59.285714285714199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>60</v>
       </c>
       <c r="B8">
         <v>62.857142857142797</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H8" s="1">
+        <v>62.857142857142797</v>
+      </c>
+      <c r="I8" s="1">
+        <v>71.428571428571402</v>
+      </c>
+      <c r="J8" s="1">
+        <v>71.428571428571402</v>
+      </c>
+      <c r="K8" s="1">
+        <v>65</v>
+      </c>
+      <c r="L8" s="1">
+        <v>64.285714285714207</v>
+      </c>
+      <c r="M8" s="1">
+        <v>62.142857142857103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>67.142857142857096</v>
       </c>
       <c r="B9">
         <v>67.142857142857096</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H9" s="1">
+        <v>65</v>
+      </c>
+      <c r="I9" s="1">
+        <v>65.714285714285694</v>
+      </c>
+      <c r="J9" s="1">
+        <v>64.285714285714207</v>
+      </c>
+      <c r="K9" s="1">
+        <v>61.428571428571402</v>
+      </c>
+      <c r="L9" s="1">
+        <v>71.428571428571402</v>
+      </c>
+      <c r="M9" s="1">
+        <v>56.428571428571402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>68.571428571428498</v>
       </c>
       <c r="B10">
         <v>67.857142857142804</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H10" s="1">
+        <v>63.571428571428498</v>
+      </c>
+      <c r="I10" s="1">
+        <v>70</v>
+      </c>
+      <c r="J10" s="1">
+        <v>68.571428571428498</v>
+      </c>
+      <c r="K10" s="1">
+        <v>65.714285714285694</v>
+      </c>
+      <c r="L10" s="1">
+        <v>67.857142857142804</v>
+      </c>
+      <c r="M10" s="1">
+        <v>56.428571428571402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>63.571428571428498</v>
       </c>
       <c r="B11">
         <v>67.142857142857096</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H11" s="1">
+        <v>60</v>
+      </c>
+      <c r="I11" s="1">
+        <v>62.857142857142797</v>
+      </c>
+      <c r="J11" s="1">
+        <v>67.857142857142804</v>
+      </c>
+      <c r="K11" s="1">
+        <v>67.142857142857096</v>
+      </c>
+      <c r="L11" s="1">
+        <v>70.714285714285694</v>
+      </c>
+      <c r="M11" s="1">
+        <v>63.571428571428498</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>61.428571428571402</v>
       </c>
       <c r="B12">
         <v>71.428571428571402</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H12" s="1">
+        <v>67.142857142857096</v>
+      </c>
+      <c r="I12" s="1">
+        <v>67.142857142857096</v>
+      </c>
+      <c r="J12" s="1">
+        <v>66.428571428571402</v>
+      </c>
+      <c r="K12" s="1">
+        <v>62.857142857142797</v>
+      </c>
+      <c r="L12" s="1">
+        <v>67.142857142857096</v>
+      </c>
+      <c r="M12" s="1">
+        <v>62.857142857142797</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>67.857142857142804</v>
       </c>
       <c r="B13">
         <v>71.428571428571402</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H13" s="1">
+        <v>68.571428571428498</v>
+      </c>
+      <c r="I13" s="1">
+        <v>67.857142857142804</v>
+      </c>
+      <c r="J13" s="1">
+        <v>77.142857142857096</v>
+      </c>
+      <c r="K13" s="1">
+        <v>71.428571428571402</v>
+      </c>
+      <c r="L13" s="1">
+        <v>70</v>
+      </c>
+      <c r="M13" s="1">
+        <v>62.142857142857103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>69.285714285714207</v>
       </c>
       <c r="B14">
         <v>68.571428571428498</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H14" s="1">
+        <v>63.571428571428498</v>
+      </c>
+      <c r="I14" s="1">
+        <v>67.142857142857096</v>
+      </c>
+      <c r="J14" s="1">
+        <v>70</v>
+      </c>
+      <c r="K14" s="1">
+        <v>68.571428571428498</v>
+      </c>
+      <c r="L14" s="1">
+        <v>61.428571428571402</v>
+      </c>
+      <c r="M14" s="1">
+        <v>55.714285714285701</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>73.571428571428498</v>
       </c>
       <c r="B15">
         <v>68.571428571428498</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H15" s="1">
+        <v>61.428571428571402</v>
+      </c>
+      <c r="I15" s="1">
+        <v>71.428571428571402</v>
+      </c>
+      <c r="J15" s="1">
+        <v>69.285714285714207</v>
+      </c>
+      <c r="K15" s="1">
+        <v>70.714285714285694</v>
+      </c>
+      <c r="L15" s="1">
+        <v>61.428571428571402</v>
+      </c>
+      <c r="M15" s="1">
+        <v>60.714285714285701</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>70</v>
       </c>
       <c r="B16">
         <v>64.285714285714207</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H16" s="1">
+        <v>67.857142857142804</v>
+      </c>
+      <c r="I16" s="1">
+        <v>71.428571428571402</v>
+      </c>
+      <c r="J16" s="1">
+        <v>60.714285714285701</v>
+      </c>
+      <c r="K16" s="1">
+        <v>67.142857142857096</v>
+      </c>
+      <c r="L16" s="1">
+        <v>72.142857142857096</v>
+      </c>
+      <c r="M16" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>67.857142857142804</v>
       </c>
       <c r="B17">
         <v>62.142857142857103</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H17" s="1">
+        <v>69.285714285714207</v>
+      </c>
+      <c r="I17" s="1">
+        <v>68.571428571428498</v>
+      </c>
+      <c r="J17" s="1">
+        <v>70.714285714285694</v>
+      </c>
+      <c r="K17" s="1">
+        <v>65.714285714285694</v>
+      </c>
+      <c r="L17" s="1">
+        <v>72.857142857142804</v>
+      </c>
+      <c r="M17" s="1">
+        <v>57.857142857142797</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>62.857142857142797</v>
       </c>
       <c r="B18">
         <v>74.285714285714207</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H18" s="1">
+        <v>73.571428571428498</v>
+      </c>
+      <c r="I18" s="1">
+        <v>68.571428571428498</v>
+      </c>
+      <c r="J18" s="1">
+        <v>69.285714285714207</v>
+      </c>
+      <c r="K18" s="1">
+        <v>69.285714285714207</v>
+      </c>
+      <c r="L18" s="1">
+        <v>67.142857142857096</v>
+      </c>
+      <c r="M18" s="1">
+        <v>55.714285714285701</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>62.857142857142797</v>
       </c>
       <c r="B19">
         <v>61.428571428571402</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H19" s="1">
+        <v>70</v>
+      </c>
+      <c r="I19" s="1">
+        <v>64.285714285714207</v>
+      </c>
+      <c r="J19" s="1">
+        <v>66.428571428571402</v>
+      </c>
+      <c r="K19" s="1">
+        <v>69.285714285714207</v>
+      </c>
+      <c r="L19" s="1">
+        <v>66.428571428571402</v>
+      </c>
+      <c r="M19" s="1">
+        <v>59.285714285714199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>66.428571428571402</v>
       </c>
       <c r="B20">
         <v>70</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H20" s="1">
+        <v>67.857142857142804</v>
+      </c>
+      <c r="I20" s="1">
+        <v>62.142857142857103</v>
+      </c>
+      <c r="J20" s="1">
+        <v>67.857142857142804</v>
+      </c>
+      <c r="K20" s="1">
+        <v>68.571428571428498</v>
+      </c>
+      <c r="L20" s="1">
+        <v>65</v>
+      </c>
+      <c r="M20" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>71.428571428571402</v>
       </c>
       <c r="B21">
         <v>62.142857142857103</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H21" s="1">
+        <v>62.857142857142797</v>
+      </c>
+      <c r="I21" s="1">
+        <v>74.285714285714207</v>
+      </c>
+      <c r="J21" s="1">
+        <v>65</v>
+      </c>
+      <c r="K21" s="1">
+        <v>67.142857142857096</v>
+      </c>
+      <c r="L21" s="1">
+        <v>67.142857142857096</v>
+      </c>
+      <c r="M21" s="1">
+        <v>59.285714285714199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H22" s="1">
+        <v>62.857142857142797</v>
+      </c>
+      <c r="I22" s="1">
+        <v>61.428571428571402</v>
+      </c>
+      <c r="J22" s="1">
+        <v>64.285714285714207</v>
+      </c>
+      <c r="K22" s="1">
+        <v>65</v>
+      </c>
+      <c r="L22" s="1">
+        <v>62.857142857142797</v>
+      </c>
+      <c r="M22" s="1">
+        <v>60.714285714285701</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>68.571428571428498</v>
       </c>
@@ -593,8 +954,26 @@
         <f>AVERAGE(B23:B42)</f>
         <v>67.21428571428568</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H23" s="1">
+        <v>66.428571428571402</v>
+      </c>
+      <c r="I23" s="1">
+        <v>70</v>
+      </c>
+      <c r="J23" s="1">
+        <v>68.571428571428498</v>
+      </c>
+      <c r="K23" s="1">
+        <v>75.714285714285694</v>
+      </c>
+      <c r="L23" s="1">
+        <v>55.714285714285701</v>
+      </c>
+      <c r="M23" s="1">
+        <v>61.428571428571402</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>64.285714285714207</v>
       </c>
@@ -609,8 +988,26 @@
         <f>_xlfn.STDEV.S(B23:B42)</f>
         <v>3.341468768944964</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H24" s="1">
+        <v>71.428571428571402</v>
+      </c>
+      <c r="I24" s="1">
+        <v>62.142857142857103</v>
+      </c>
+      <c r="J24" s="1">
+        <v>69.285714285714207</v>
+      </c>
+      <c r="K24" s="1">
+        <v>63.571428571428498</v>
+      </c>
+      <c r="L24" s="1">
+        <v>70</v>
+      </c>
+      <c r="M24" s="1">
+        <v>52.142857142857103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>69.285714285714207</v>
       </c>
@@ -618,7 +1015,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>71.428571428571402</v>
       </c>
@@ -626,7 +1023,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>64.285714285714207</v>
       </c>
@@ -634,7 +1031,7 @@
         <v>61.428571428571402</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>68.571428571428498</v>
       </c>
@@ -642,7 +1039,7 @@
         <v>65.714285714285694</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>67.857142857142804</v>
       </c>
@@ -650,7 +1047,7 @@
         <v>67.142857142857096</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>66.428571428571402</v>
       </c>
@@ -658,7 +1055,7 @@
         <v>62.857142857142797</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>77.142857142857096</v>
       </c>
@@ -666,7 +1063,7 @@
         <v>71.428571428571402</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>70</v>
       </c>
@@ -933,6 +1330,107 @@
       </c>
       <c r="B63">
         <v>52.142857142857103</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>71.428571428571402</v>
+      </c>
+      <c r="B65">
+        <v>67.142857142857096</v>
+      </c>
+      <c r="D65">
+        <f>AVERAGE(A65:A74)</f>
+        <v>68.357142857142804</v>
+      </c>
+      <c r="E65">
+        <f>AVERAGE(B65:B74)</f>
+        <v>66.714285714285666</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>70.714285714285694</v>
+      </c>
+      <c r="B66">
+        <v>65</v>
+      </c>
+      <c r="D66">
+        <f>_xlfn.STDEV.S(A65:A74)</f>
+        <v>3.0869853349262693</v>
+      </c>
+      <c r="E66">
+        <f>_xlfn.STDEV.S(B65:B74)</f>
+        <v>3.7525501533039014</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>67.142857142857096</v>
+      </c>
+      <c r="B67">
+        <v>71.428571428571402</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>73.571428571428498</v>
+      </c>
+      <c r="B68">
+        <v>72.857142857142804</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>63.571428571428498</v>
+      </c>
+      <c r="B69">
+        <v>67.857142857142804</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>69.285714285714207</v>
+      </c>
+      <c r="B70">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>65.714285714285694</v>
+      </c>
+      <c r="B71">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>65</v>
+      </c>
+      <c r="B72">
+        <v>65.714285714285694</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>68.571428571428498</v>
+      </c>
+      <c r="B73">
+        <v>68.571428571428498</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>68.571428571428498</v>
+      </c>
+      <c r="B74">
+        <v>63.571428571428498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>